<commit_message>
updated model, added weir fun, and included draft write-up methods
</commit_message>
<xml_diff>
--- a/data/trib_data/lostine.xlsx
+++ b/data/trib_data/lostine.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub_Repos\Save-the-Salmon-Models\data\trib_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub_Repos\Chinook-Life-Cycle\data\trib_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AD1E851-E446-410F-80CD-B0303410E745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FDB33E-42F1-47E2-9FC3-C7A02488FA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="5025" windowWidth="40770" windowHeight="20010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="2115" windowWidth="22005" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -442,7 +442,7 @@
   <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +456,12 @@
     <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="18" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="10" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" customWidth="1"/>
+    <col min="17" max="17" width="7.85546875" customWidth="1"/>
+    <col min="18" max="18" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1345,10 +1350,10 @@
         <v>171105</v>
       </c>
       <c r="M17">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="N17">
-        <v>1300</v>
+        <v>1271</v>
       </c>
       <c r="O17">
         <v>77</v>
@@ -1401,7 +1406,7 @@
         <v>159023</v>
       </c>
       <c r="M18">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="N18">
         <v>551</v>
@@ -1525,7 +1530,7 @@
         <v>171</v>
       </c>
       <c r="Q20">
-        <v>607</v>
+        <v>519</v>
       </c>
       <c r="R20">
         <v>37</v>
@@ -1572,16 +1577,16 @@
         <v>17</v>
       </c>
       <c r="N21">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="O21">
         <v>19</v>
       </c>
       <c r="P21">
-        <v>88</v>
+        <v>177</v>
       </c>
       <c r="Q21">
-        <v>757</v>
+        <v>726</v>
       </c>
       <c r="R21">
         <v>67</v>
@@ -1625,16 +1630,16 @@
         <v>150961</v>
       </c>
       <c r="M22">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="N22">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="O22">
         <v>4</v>
       </c>
       <c r="P22">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="Q22">
         <v>356</v>
@@ -1681,19 +1686,19 @@
         <v>147486</v>
       </c>
       <c r="M23">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="N23">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="O23">
         <v>0</v>
       </c>
       <c r="P23">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="Q23">
-        <v>748</v>
+        <v>591</v>
       </c>
       <c r="R23">
         <v>11</v>
@@ -1737,7 +1742,7 @@
         <v>146442</v>
       </c>
       <c r="M24">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="N24">
         <v>157</v>
@@ -1746,10 +1751,10 @@
         <v>33</v>
       </c>
       <c r="P24">
-        <v>52</v>
+        <v>209</v>
       </c>
       <c r="Q24">
-        <v>654</v>
+        <v>586</v>
       </c>
       <c r="R24">
         <v>22</v>
@@ -1802,7 +1807,7 @@
         <v>0</v>
       </c>
       <c r="P25">
-        <v>68</v>
+        <v>137</v>
       </c>
       <c r="Q25">
         <v>741</v>

</xml_diff>